<commit_message>
relatorio de andamentos convertendo xls
</commit_message>
<xml_diff>
--- a/excel files/convertido-geral.xlsx
+++ b/excel files/convertido-geral.xlsx
@@ -68,7 +68,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -80,9 +80,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -450,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,409 +455,387 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16.47" customWidth="1" min="1" max="1"/>
-    <col width="17.53666666666667" customWidth="1" min="2" max="2"/>
-    <col width="15.67" customWidth="1" min="3" max="3"/>
-    <col width="23.40333333333333" customWidth="1" min="4" max="4"/>
-    <col width="33.80333333333333" customWidth="1" min="5" max="5"/>
-    <col width="28.47" customWidth="1" min="6" max="6"/>
-    <col width="23.93666666666667" customWidth="1" min="7" max="7"/>
-    <col width="38.87" customWidth="1" min="8" max="8"/>
-    <col width="32.20333333333333" customWidth="1" min="9" max="9"/>
-    <col width="29.28142857142857" customWidth="1" min="10" max="10"/>
-    <col width="20.20333333333333" customWidth="1" min="11" max="11"/>
-    <col width="38.33666666666667" customWidth="1" min="12" max="12"/>
-    <col width="23.67" customWidth="1" min="13" max="13"/>
-    <col width="20.73666666666667" customWidth="1" min="14" max="14"/>
-    <col width="48.76333333333334" customWidth="1" min="15" max="15"/>
-    <col width="58.36333333333333" customWidth="1" min="16" max="16"/>
-    <col width="30.60333333333334" customWidth="1" min="17" max="17"/>
-    <col width="41.02999999999999" customWidth="1" min="18" max="18"/>
-    <col width="43.43000000000001" customWidth="1" min="19" max="19"/>
+    <col width="23.32333333333333" customWidth="1" min="1" max="1"/>
+    <col width="15.77666666666667" customWidth="1" min="2" max="2"/>
+    <col width="23.32333333333333" customWidth="1" min="3" max="3"/>
+    <col width="28.41666666666667" customWidth="1" min="4" max="4"/>
+    <col width="25.45666666666667" customWidth="1" min="5" max="5"/>
+    <col width="19.80333333333333" customWidth="1" min="6" max="6"/>
+    <col width="30.84333333333334" customWidth="1" min="7" max="7"/>
+    <col width="32.73666666666666" customWidth="1" min="8" max="8"/>
+    <col width="26.28333333333333" customWidth="1" min="9" max="9"/>
+    <col width="19.80333333333333" customWidth="1" min="10" max="10"/>
+    <col width="28.68333333333334" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.5" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Status</t>
+          <t>Concluida</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Pedido</t>
+          <t>Ação</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>Acao Tipo</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Acao Tipo</t>
+          <t>Responsável</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Envolvidos</t>
+          <t>Agente</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Responsável</t>
+          <t>Contato</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Valor Total</t>
+          <t>Data Cadastro</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Fornecedor Master</t>
+          <t>Data</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Data Início</t>
+          <t>Tempo(Min)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Data Termino</t>
+          <t>Produto</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Duração</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Último Andamento</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Prioridade</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Forecast</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Agente</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
           <t>Descrição</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Ñ.Fech Motivo</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Ñ.Fech Concorrente</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Ñ.Fech Detalhamento</t>
-        </is>
-      </c>
     </row>
-    <row r="2" ht="78" customHeight="1">
+    <row r="2" ht="65.5" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Aberta</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr"/>
-      <c r="C2" s="3" t="n">
-        <v>22649</v>
+          <t>emaberto</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>20376</v>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Serviços</t>
+        </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>Suporte Técnico</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>Yasmim</t>
+          <t>Vitor Pereira Diogo</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>SGMP - Schneebeli, Gimenes, Moraes e Pepe Advogado...</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>Yasmim</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="inlineStr"/>
-      <c r="H2" s="2" t="inlineStr"/>
-      <c r="I2" s="4" t="n">
-        <v>44372</v>
+          <t>SJ</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>44390</v>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>13/07/2021 | 16:30:00 a 16:44:00</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>14</v>
       </c>
       <c r="J2" s="2" t="inlineStr"/>
       <c r="K2" s="2" t="inlineStr">
         <is>
-          <t>3 dias</t>
-        </is>
-      </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>4 dias atrás</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="N2" s="5" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="O2" s="3" t="inlineStr">
-        <is>
-          <t>Francisco Domingos Vieira Advogados Associados</t>
-        </is>
-      </c>
-      <c r="P2" s="2" t="inlineStr">
-        <is>
-          <t>TR - Karen entrou em contato informando que não estava conseguindo abrir o cp pro, pedi que ela me mandasse imagem do erro por ema...</t>
-        </is>
-      </c>
-      <c r="Q2" s="2" t="inlineStr"/>
-      <c r="R2" s="2" t="inlineStr"/>
-      <c r="S2" s="2" t="inlineStr"/>
+          <t>Análise e teste de WF para o cliente. Elaboração de esboço do fluxo para teste. ...</t>
+        </is>
+      </c>
     </row>
-    <row r="3" ht="78" customHeight="1">
+    <row r="3" ht="65.5" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Aberta</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr"/>
-      <c r="C3" s="3" t="n">
-        <v>22646</v>
+          <t>emaberto</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>22793</v>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Serviços</t>
+        </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>Suporte Técnico</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>Yasmim</t>
+          <t>Vitor Pereira Diogo</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>Eliane Matos Pires</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>Yasmim</t>
-        </is>
-      </c>
-      <c r="G3" s="2" t="inlineStr"/>
-      <c r="H3" s="2" t="inlineStr"/>
-      <c r="I3" s="4" t="n">
-        <v>44372</v>
+          <t>Bruno</t>
+        </is>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>44390</v>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>13/07/2021 | 10:50:00 a 11:15:00</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>25</v>
       </c>
       <c r="J3" s="2" t="inlineStr"/>
       <c r="K3" s="2" t="inlineStr">
         <is>
-          <t>4 dias</t>
-        </is>
-      </c>
-      <c r="L3" s="2" t="inlineStr">
-        <is>
-          <t>4 dias atrás</t>
-        </is>
-      </c>
-      <c r="M3" s="2" t="inlineStr">
-        <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="N3" s="5" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="O3" s="3" t="inlineStr">
+          <t>Bruno me informou que não consegue passar o acesso remoto ao servidor para que e...</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="65.5" customHeight="1">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>fechado</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>22784</v>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Suporte Funcional</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Vitor Pereira Diogo</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>Oliveira Cardoso, Carvalho de Brito, Libardi Comar...</t>
         </is>
       </c>
-      <c r="P3" s="2" t="inlineStr">
-        <is>
-          <t>TR - Cliente entrou em contato informando grande lentidão no sistema. Abri suporte com a Thomson, número do caso: 07755601.</t>
-        </is>
-      </c>
-      <c r="Q3" s="2" t="inlineStr"/>
-      <c r="R3" s="2" t="inlineStr"/>
-      <c r="S3" s="2" t="inlineStr"/>
-    </row>
-    <row r="4" ht="78" customHeight="1">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Aberta</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr"/>
-      <c r="C4" s="3" t="n">
-        <v>22645</v>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>Suporte Técnico</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>Yasmim</t>
-        </is>
-      </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>Yasmim</t>
-        </is>
-      </c>
-      <c r="G4" s="2" t="inlineStr"/>
-      <c r="H4" s="2" t="inlineStr"/>
-      <c r="I4" s="4" t="n">
-        <v>44372</v>
+          <t>SJ</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>44390</v>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>13/07/2021 | 10:35:00 a 10:48:00</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>13</v>
       </c>
       <c r="J4" s="2" t="inlineStr"/>
       <c r="K4" s="2" t="inlineStr">
         <is>
-          <t>4 dias</t>
-        </is>
-      </c>
-      <c r="L4" s="2" t="inlineStr">
-        <is>
-          <t>4 dias atrás</t>
-        </is>
-      </c>
-      <c r="M4" s="2" t="inlineStr">
-        <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="N4" s="5" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="O4" s="3" t="inlineStr">
-        <is>
-          <t>SGMP - Schneebeli, Gimenes, Moraes e Pepe Advogado...</t>
-        </is>
-      </c>
-      <c r="P4" s="2" t="inlineStr">
-        <is>
-          <t>TR - Cliente entrou em contato informando grande lentidão no sistema. Abri suporte com a Thomson, número do caso: 07755530.</t>
-        </is>
-      </c>
-      <c r="Q4" s="2" t="inlineStr"/>
-      <c r="R4" s="2" t="inlineStr"/>
-      <c r="S4" s="2" t="inlineStr"/>
+          <t>Em contato com Vanessa e Stephanie, fizemos as configurações e confirmamos que o...</t>
+        </is>
+      </c>
     </row>
-    <row r="5" ht="78" customHeight="1">
+    <row r="5" ht="65.5" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Aberta</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr"/>
-      <c r="C5" s="3" t="n">
-        <v>22618</v>
+          <t>fechado</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>22784</v>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Suporte Funcional</t>
+        </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>Suporte Técnico</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
           <t>Vitor Pereira Diogo</t>
         </is>
       </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>Oliveira Cardoso, Carvalho de Brito, Libardi Comar...</t>
+        </is>
+      </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>Vitor Pereira Diogo</t>
-        </is>
-      </c>
-      <c r="G5" s="2" t="inlineStr"/>
-      <c r="H5" s="2" t="inlineStr"/>
-      <c r="I5" s="4" t="n">
-        <v>44368</v>
+          <t>Deborah</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>44390</v>
+      </c>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>13/07/2021 | 09:35:00 a 09:35:00</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="J5" s="2" t="inlineStr"/>
       <c r="K5" s="2" t="inlineStr">
         <is>
-          <t>7 dias</t>
-        </is>
-      </c>
-      <c r="L5" s="2" t="inlineStr">
-        <is>
-          <t>8 dias atrás</t>
-        </is>
-      </c>
-      <c r="M5" s="2" t="inlineStr">
-        <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="N5" s="5" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="O5" s="3" t="inlineStr">
-        <is>
-          <t>Zouain, Rizk &amp; Advogados Associados</t>
-        </is>
-      </c>
-      <c r="P5" s="2" t="inlineStr">
-        <is>
-          <t>Vitor Diogo &lt;suporte@shopjuridico.com.br&gt; 17:45 (há 4 minutos) para giselli.fonseca, Priscila, Suporte1 Prezada Giselli, boa ...</t>
-        </is>
-      </c>
-      <c r="Q5" s="2" t="inlineStr"/>
-      <c r="R5" s="2" t="inlineStr"/>
-      <c r="S5" s="2" t="inlineStr"/>
+          <t>Deborah da Silva Faria Borges Barbosa 09:35 (há 50 minutos) para mim, Stephani...</t>
+        </is>
+      </c>
     </row>
-    <row r="6" ht="15.5" customHeight="1">
-      <c r="A6" s="2" t="inlineStr"/>
-      <c r="B6" s="2" t="inlineStr"/>
-      <c r="C6" s="2" t="inlineStr"/>
-      <c r="D6" s="2" t="inlineStr"/>
-      <c r="E6" s="2" t="inlineStr"/>
-      <c r="F6" s="2" t="inlineStr"/>
-      <c r="G6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="inlineStr"/>
-      <c r="I6" s="2" t="inlineStr"/>
+    <row r="6" ht="65.5" customHeight="1">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>fechado</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>22784</v>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Suporte Funcional</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>Vitor Pereira Diogo</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>Oliveira Cardoso, Carvalho de Brito, Libardi Comar...</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>Deborah</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>44390</v>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>13/07/2021 | 09:18:00 a 09:33:00</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>15</v>
+      </c>
       <c r="J6" s="2" t="inlineStr"/>
-      <c r="K6" s="2" t="inlineStr"/>
-      <c r="L6" s="2" t="inlineStr"/>
-      <c r="M6" s="2" t="inlineStr"/>
-      <c r="N6" s="2" t="inlineStr"/>
-      <c r="O6" s="2" t="inlineStr"/>
-      <c r="P6" s="2" t="inlineStr"/>
-      <c r="Q6" s="2" t="inlineStr"/>
-      <c r="R6" s="2" t="inlineStr"/>
-      <c r="S6" s="2" t="inlineStr"/>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>[09:18, 13/07/2021] Vitor Diogo: ei, Deborah [09:18, 13/07/2021] Vitor Diogo: a...</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="65.5" customHeight="1">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>fechado</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>22784</v>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Suporte Funcional</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Vitor Pereira Diogo</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>Oliveira Cardoso, Carvalho de Brito, Libardi Comar...</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>Deborah</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>44390</v>
+      </c>
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>13/07/2021 | 08:48:00 a 08:51:00</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J7" s="2" t="inlineStr"/>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>Bom dia, Deborah! Tudo certinho? Conforme o retorno na sexta-feira, é precis...</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="15.5" customHeight="1">
+      <c r="A8" s="2" t="inlineStr"/>
+      <c r="B8" s="2" t="inlineStr"/>
+      <c r="C8" s="2" t="inlineStr"/>
+      <c r="D8" s="2" t="inlineStr"/>
+      <c r="E8" s="2" t="inlineStr"/>
+      <c r="F8" s="2" t="inlineStr"/>
+      <c r="G8" s="2" t="inlineStr"/>
+      <c r="H8" s="2" t="inlineStr"/>
+      <c r="I8" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="J8" s="2" t="inlineStr"/>
+      <c r="K8" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="O2" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="O3" r:id="rId4"/>
-    <hyperlink ref="C4" r:id="rId5"/>
-    <hyperlink ref="O4" r:id="rId6"/>
-    <hyperlink ref="C5" r:id="rId7"/>
-    <hyperlink ref="O5" r:id="rId8"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="E4" r:id="rId6"/>
+    <hyperlink ref="B5" r:id="rId7"/>
+    <hyperlink ref="E5" r:id="rId8"/>
+    <hyperlink ref="B6" r:id="rId9"/>
+    <hyperlink ref="E6" r:id="rId10"/>
+    <hyperlink ref="B7" r:id="rId11"/>
+    <hyperlink ref="E7" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>